<commit_message>
FIX:Correct typo in Broader IRI
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="684">
   <si>
     <t xml:space="preserve">ConceptScheme URI</t>
   </si>
@@ -1238,9 +1238,6 @@
   </si>
   <si>
     <t xml:space="preserve">Air Termination</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reliatax:Lightning Protection System</t>
   </si>
   <si>
     <t xml:space="preserve">reliatax:AuxiliaryElectricalSystemLightningProtectionSystemBondingElement</t>
@@ -2532,8 +2529,8 @@
   </sheetPr>
   <dimension ref="A1:I359"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A207" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F206" activeCellId="0" sqref="F206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4878,78 +4875,78 @@
         <v>405</v>
       </c>
       <c r="E206" s="12" t="s">
-        <v>406</v>
+        <v>136</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A207" s="12" t="s">
+        <v>406</v>
+      </c>
+      <c r="B207" s="12" t="s">
         <v>407</v>
       </c>
-      <c r="B207" s="12" t="s">
-        <v>408</v>
-      </c>
       <c r="E207" s="12" t="s">
-        <v>406</v>
+        <v>136</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A208" s="12" t="s">
+        <v>408</v>
+      </c>
+      <c r="B208" s="12" t="s">
         <v>409</v>
       </c>
-      <c r="B208" s="12" t="s">
-        <v>410</v>
-      </c>
       <c r="E208" s="12" t="s">
-        <v>406</v>
+        <v>136</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A209" s="12" t="s">
+        <v>410</v>
+      </c>
+      <c r="B209" s="12" t="s">
         <v>411</v>
       </c>
-      <c r="B209" s="12" t="s">
-        <v>412</v>
-      </c>
       <c r="E209" s="12" t="s">
-        <v>406</v>
+        <v>136</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A210" s="12" t="s">
+        <v>412</v>
+      </c>
+      <c r="B210" s="12" t="s">
         <v>413</v>
       </c>
-      <c r="B210" s="12" t="s">
-        <v>414</v>
-      </c>
       <c r="E210" s="12" t="s">
-        <v>406</v>
+        <v>136</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A211" s="12" t="s">
+        <v>414</v>
+      </c>
+      <c r="B211" s="12" t="s">
         <v>415</v>
       </c>
-      <c r="B211" s="12" t="s">
-        <v>416</v>
-      </c>
       <c r="E211" s="12" t="s">
-        <v>406</v>
+        <v>136</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A212" s="12" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B212" s="12" t="s">
         <v>399</v>
       </c>
       <c r="E212" s="12" t="s">
-        <v>406</v>
+        <v>136</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A213" s="12" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B213" s="12" t="s">
         <v>375</v>
@@ -4960,10 +4957,10 @@
     </row>
     <row r="214" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A214" s="12" t="s">
+        <v>418</v>
+      </c>
+      <c r="B214" s="12" t="s">
         <v>419</v>
-      </c>
-      <c r="B214" s="12" t="s">
-        <v>420</v>
       </c>
       <c r="E214" s="12" t="s">
         <v>138</v>
@@ -4971,10 +4968,10 @@
     </row>
     <row r="215" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A215" s="12" t="s">
+        <v>420</v>
+      </c>
+      <c r="B215" s="12" t="s">
         <v>421</v>
-      </c>
-      <c r="B215" s="12" t="s">
-        <v>422</v>
       </c>
       <c r="E215" s="12" t="s">
         <v>138</v>
@@ -4982,10 +4979,10 @@
     </row>
     <row r="216" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A216" s="12" t="s">
+        <v>422</v>
+      </c>
+      <c r="B216" s="12" t="s">
         <v>423</v>
-      </c>
-      <c r="B216" s="12" t="s">
-        <v>424</v>
       </c>
       <c r="E216" s="12" t="s">
         <v>138</v>
@@ -4993,10 +4990,10 @@
     </row>
     <row r="217" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A217" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="B217" s="12" t="s">
         <v>425</v>
-      </c>
-      <c r="B217" s="12" t="s">
-        <v>426</v>
       </c>
       <c r="E217" s="12" t="s">
         <v>140</v>
@@ -5004,10 +5001,10 @@
     </row>
     <row r="218" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A218" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="B218" s="12" t="s">
         <v>427</v>
-      </c>
-      <c r="B218" s="12" t="s">
-        <v>428</v>
       </c>
       <c r="E218" s="12" t="s">
         <v>140</v>
@@ -5015,10 +5012,10 @@
     </row>
     <row r="219" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A219" s="12" t="s">
+        <v>428</v>
+      </c>
+      <c r="B219" s="12" t="s">
         <v>429</v>
-      </c>
-      <c r="B219" s="12" t="s">
-        <v>430</v>
       </c>
       <c r="E219" s="12" t="s">
         <v>140</v>
@@ -5026,10 +5023,10 @@
     </row>
     <row r="220" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A220" s="12" t="s">
+        <v>430</v>
+      </c>
+      <c r="B220" s="12" t="s">
         <v>431</v>
-      </c>
-      <c r="B220" s="12" t="s">
-        <v>432</v>
       </c>
       <c r="E220" s="12" t="s">
         <v>140</v>
@@ -5037,10 +5034,10 @@
     </row>
     <row r="221" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A221" s="12" t="s">
+        <v>432</v>
+      </c>
+      <c r="B221" s="12" t="s">
         <v>433</v>
-      </c>
-      <c r="B221" s="12" t="s">
-        <v>434</v>
       </c>
       <c r="E221" s="12" t="s">
         <v>140</v>
@@ -5048,10 +5045,10 @@
     </row>
     <row r="222" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A222" s="12" t="s">
+        <v>434</v>
+      </c>
+      <c r="B222" s="12" t="s">
         <v>435</v>
-      </c>
-      <c r="B222" s="12" t="s">
-        <v>436</v>
       </c>
       <c r="E222" s="12" t="s">
         <v>140</v>
@@ -5059,10 +5056,10 @@
     </row>
     <row r="223" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A223" s="12" t="s">
+        <v>436</v>
+      </c>
+      <c r="B223" s="12" t="s">
         <v>437</v>
-      </c>
-      <c r="B223" s="12" t="s">
-        <v>438</v>
       </c>
       <c r="E223" s="12" t="s">
         <v>142</v>
@@ -5070,10 +5067,10 @@
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A224" s="12" t="s">
+        <v>438</v>
+      </c>
+      <c r="B224" s="12" t="s">
         <v>439</v>
-      </c>
-      <c r="B224" s="12" t="s">
-        <v>440</v>
       </c>
       <c r="E224" s="12" t="s">
         <v>142</v>
@@ -5081,10 +5078,10 @@
     </row>
     <row r="225" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A225" s="12" t="s">
+        <v>440</v>
+      </c>
+      <c r="B225" s="12" t="s">
         <v>441</v>
-      </c>
-      <c r="B225" s="12" t="s">
-        <v>442</v>
       </c>
       <c r="E225" s="12" t="s">
         <v>142</v>
@@ -5092,10 +5089,10 @@
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A226" s="12" t="s">
+        <v>442</v>
+      </c>
+      <c r="B226" s="12" t="s">
         <v>443</v>
-      </c>
-      <c r="B226" s="12" t="s">
-        <v>444</v>
       </c>
       <c r="E226" s="12" t="s">
         <v>142</v>
@@ -5103,10 +5100,10 @@
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A227" s="12" t="s">
+        <v>444</v>
+      </c>
+      <c r="B227" s="12" t="s">
         <v>445</v>
-      </c>
-      <c r="B227" s="12" t="s">
-        <v>446</v>
       </c>
       <c r="E227" s="12" t="s">
         <v>144</v>
@@ -5114,10 +5111,10 @@
     </row>
     <row r="228" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A228" s="12" t="s">
+        <v>446</v>
+      </c>
+      <c r="B228" s="12" t="s">
         <v>447</v>
-      </c>
-      <c r="B228" s="12" t="s">
-        <v>448</v>
       </c>
       <c r="E228" s="12" t="s">
         <v>144</v>
@@ -5125,10 +5122,10 @@
     </row>
     <row r="229" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A229" s="12" t="s">
+        <v>448</v>
+      </c>
+      <c r="B229" s="12" t="s">
         <v>449</v>
-      </c>
-      <c r="B229" s="12" t="s">
-        <v>450</v>
       </c>
       <c r="E229" s="12" t="s">
         <v>144</v>
@@ -5136,10 +5133,10 @@
     </row>
     <row r="230" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A230" s="12" t="s">
+        <v>450</v>
+      </c>
+      <c r="B230" s="12" t="s">
         <v>451</v>
-      </c>
-      <c r="B230" s="12" t="s">
-        <v>452</v>
       </c>
       <c r="E230" s="12" t="s">
         <v>144</v>
@@ -5147,10 +5144,10 @@
     </row>
     <row r="231" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A231" s="12" t="s">
+        <v>452</v>
+      </c>
+      <c r="B231" s="12" t="s">
         <v>453</v>
-      </c>
-      <c r="B231" s="12" t="s">
-        <v>454</v>
       </c>
       <c r="E231" s="12" t="s">
         <v>144</v>
@@ -5158,10 +5155,10 @@
     </row>
     <row r="232" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A232" s="12" t="s">
+        <v>454</v>
+      </c>
+      <c r="B232" s="12" t="s">
         <v>455</v>
-      </c>
-      <c r="B232" s="12" t="s">
-        <v>456</v>
       </c>
       <c r="E232" s="12" t="s">
         <v>146</v>
@@ -5169,10 +5166,10 @@
     </row>
     <row r="233" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A233" s="12" t="s">
+        <v>456</v>
+      </c>
+      <c r="B233" s="12" t="s">
         <v>457</v>
-      </c>
-      <c r="B233" s="12" t="s">
-        <v>458</v>
       </c>
       <c r="E233" s="12" t="s">
         <v>146</v>
@@ -5180,10 +5177,10 @@
     </row>
     <row r="234" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A234" s="12" t="s">
+        <v>458</v>
+      </c>
+      <c r="B234" s="12" t="s">
         <v>459</v>
-      </c>
-      <c r="B234" s="12" t="s">
-        <v>460</v>
       </c>
       <c r="E234" s="12" t="s">
         <v>148</v>
@@ -5191,10 +5188,10 @@
     </row>
     <row r="235" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A235" s="12" t="s">
+        <v>460</v>
+      </c>
+      <c r="B235" s="12" t="s">
         <v>461</v>
-      </c>
-      <c r="B235" s="12" t="s">
-        <v>462</v>
       </c>
       <c r="E235" s="12" t="s">
         <v>148</v>
@@ -5202,10 +5199,10 @@
     </row>
     <row r="236" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A236" s="12" t="s">
+        <v>462</v>
+      </c>
+      <c r="B236" s="12" t="s">
         <v>463</v>
-      </c>
-      <c r="B236" s="12" t="s">
-        <v>464</v>
       </c>
       <c r="E236" s="12" t="s">
         <v>148</v>
@@ -5213,10 +5210,10 @@
     </row>
     <row r="237" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A237" s="12" t="s">
+        <v>464</v>
+      </c>
+      <c r="B237" s="12" t="s">
         <v>465</v>
-      </c>
-      <c r="B237" s="12" t="s">
-        <v>466</v>
       </c>
       <c r="E237" s="12" t="s">
         <v>148</v>
@@ -5224,10 +5221,10 @@
     </row>
     <row r="238" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A238" s="12" t="s">
+        <v>466</v>
+      </c>
+      <c r="B238" s="12" t="s">
         <v>467</v>
-      </c>
-      <c r="B238" s="12" t="s">
-        <v>468</v>
       </c>
       <c r="E238" s="12" t="s">
         <v>148</v>
@@ -5235,10 +5232,10 @@
     </row>
     <row r="239" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A239" s="12" t="s">
+        <v>468</v>
+      </c>
+      <c r="B239" s="12" t="s">
         <v>469</v>
-      </c>
-      <c r="B239" s="12" t="s">
-        <v>470</v>
       </c>
       <c r="E239" s="12" t="s">
         <v>148</v>
@@ -5246,10 +5243,10 @@
     </row>
     <row r="240" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A240" s="12" t="s">
+        <v>470</v>
+      </c>
+      <c r="B240" s="12" t="s">
         <v>471</v>
-      </c>
-      <c r="B240" s="12" t="s">
-        <v>472</v>
       </c>
       <c r="E240" s="12" t="s">
         <v>148</v>
@@ -5257,10 +5254,10 @@
     </row>
     <row r="241" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A241" s="12" t="s">
+        <v>472</v>
+      </c>
+      <c r="B241" s="12" t="s">
         <v>473</v>
-      </c>
-      <c r="B241" s="12" t="s">
-        <v>474</v>
       </c>
       <c r="E241" s="12" t="s">
         <v>150</v>
@@ -5268,7 +5265,7 @@
     </row>
     <row r="242" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A242" s="12" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B242" s="12" t="s">
         <v>377</v>
@@ -5279,10 +5276,10 @@
     </row>
     <row r="243" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A243" s="12" t="s">
+        <v>475</v>
+      </c>
+      <c r="B243" s="12" t="s">
         <v>476</v>
-      </c>
-      <c r="B243" s="12" t="s">
-        <v>477</v>
       </c>
       <c r="E243" s="12" t="s">
         <v>150</v>
@@ -5290,10 +5287,10 @@
     </row>
     <row r="244" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A244" s="12" t="s">
+        <v>477</v>
+      </c>
+      <c r="B244" s="12" t="s">
         <v>478</v>
-      </c>
-      <c r="B244" s="12" t="s">
-        <v>479</v>
       </c>
       <c r="E244" s="12" t="s">
         <v>150</v>
@@ -5301,10 +5298,10 @@
     </row>
     <row r="245" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A245" s="12" t="s">
+        <v>479</v>
+      </c>
+      <c r="B245" s="12" t="s">
         <v>480</v>
-      </c>
-      <c r="B245" s="12" t="s">
-        <v>481</v>
       </c>
       <c r="E245" s="12" t="s">
         <v>150</v>
@@ -5312,10 +5309,10 @@
     </row>
     <row r="246" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A246" s="12" t="s">
+        <v>481</v>
+      </c>
+      <c r="B246" s="12" t="s">
         <v>482</v>
-      </c>
-      <c r="B246" s="12" t="s">
-        <v>483</v>
       </c>
       <c r="E246" s="12" t="s">
         <v>150</v>
@@ -5323,10 +5320,10 @@
     </row>
     <row r="247" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A247" s="12" t="s">
+        <v>483</v>
+      </c>
+      <c r="B247" s="12" t="s">
         <v>484</v>
-      </c>
-      <c r="B247" s="12" t="s">
-        <v>485</v>
       </c>
       <c r="E247" s="12" t="s">
         <v>150</v>
@@ -5334,10 +5331,10 @@
     </row>
     <row r="248" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A248" s="12" t="s">
+        <v>485</v>
+      </c>
+      <c r="B248" s="12" t="s">
         <v>486</v>
-      </c>
-      <c r="B248" s="12" t="s">
-        <v>487</v>
       </c>
       <c r="E248" s="12" t="s">
         <v>150</v>
@@ -5345,10 +5342,10 @@
     </row>
     <row r="249" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A249" s="12" t="s">
+        <v>487</v>
+      </c>
+      <c r="B249" s="12" t="s">
         <v>488</v>
-      </c>
-      <c r="B249" s="12" t="s">
-        <v>489</v>
       </c>
       <c r="E249" s="12" t="s">
         <v>150</v>
@@ -5356,10 +5353,10 @@
     </row>
     <row r="250" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A250" s="12" t="s">
+        <v>489</v>
+      </c>
+      <c r="B250" s="12" t="s">
         <v>490</v>
-      </c>
-      <c r="B250" s="12" t="s">
-        <v>491</v>
       </c>
       <c r="E250" s="12" t="s">
         <v>150</v>
@@ -5367,10 +5364,10 @@
     </row>
     <row r="251" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A251" s="12" t="s">
+        <v>491</v>
+      </c>
+      <c r="B251" s="12" t="s">
         <v>492</v>
-      </c>
-      <c r="B251" s="12" t="s">
-        <v>493</v>
       </c>
       <c r="E251" s="12" t="s">
         <v>150</v>
@@ -5378,10 +5375,10 @@
     </row>
     <row r="252" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A252" s="12" t="s">
+        <v>493</v>
+      </c>
+      <c r="B252" s="12" t="s">
         <v>494</v>
-      </c>
-      <c r="B252" s="12" t="s">
-        <v>495</v>
       </c>
       <c r="E252" s="12" t="s">
         <v>150</v>
@@ -5389,10 +5386,10 @@
     </row>
     <row r="253" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A253" s="12" t="s">
+        <v>495</v>
+      </c>
+      <c r="B253" s="12" t="s">
         <v>496</v>
-      </c>
-      <c r="B253" s="12" t="s">
-        <v>497</v>
       </c>
       <c r="E253" s="12" t="s">
         <v>150</v>
@@ -5400,10 +5397,10 @@
     </row>
     <row r="254" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A254" s="12" t="s">
+        <v>497</v>
+      </c>
+      <c r="B254" s="12" t="s">
         <v>498</v>
-      </c>
-      <c r="B254" s="12" t="s">
-        <v>499</v>
       </c>
       <c r="E254" s="12" t="s">
         <v>152</v>
@@ -5411,10 +5408,10 @@
     </row>
     <row r="255" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A255" s="12" t="s">
+        <v>499</v>
+      </c>
+      <c r="B255" s="12" t="s">
         <v>500</v>
-      </c>
-      <c r="B255" s="12" t="s">
-        <v>501</v>
       </c>
       <c r="E255" s="12" t="s">
         <v>152</v>
@@ -5422,10 +5419,10 @@
     </row>
     <row r="256" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A256" s="12" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B256" s="12" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E256" s="12" t="s">
         <v>152</v>
@@ -5433,10 +5430,10 @@
     </row>
     <row r="257" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A257" s="12" t="s">
+        <v>502</v>
+      </c>
+      <c r="B257" s="12" t="s">
         <v>503</v>
-      </c>
-      <c r="B257" s="12" t="s">
-        <v>504</v>
       </c>
       <c r="E257" s="12" t="s">
         <v>152</v>
@@ -5444,10 +5441,10 @@
     </row>
     <row r="258" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A258" s="12" t="s">
+        <v>504</v>
+      </c>
+      <c r="B258" s="12" t="s">
         <v>505</v>
-      </c>
-      <c r="B258" s="12" t="s">
-        <v>506</v>
       </c>
       <c r="E258" s="12" t="s">
         <v>152</v>
@@ -5455,10 +5452,10 @@
     </row>
     <row r="259" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A259" s="12" t="s">
+        <v>506</v>
+      </c>
+      <c r="B259" s="12" t="s">
         <v>507</v>
-      </c>
-      <c r="B259" s="12" t="s">
-        <v>508</v>
       </c>
       <c r="E259" s="12" t="s">
         <v>152</v>
@@ -5466,10 +5463,10 @@
     </row>
     <row r="260" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A260" s="12" t="s">
+        <v>508</v>
+      </c>
+      <c r="B260" s="12" t="s">
         <v>509</v>
-      </c>
-      <c r="B260" s="12" t="s">
-        <v>510</v>
       </c>
       <c r="E260" s="12" t="s">
         <v>152</v>
@@ -5477,10 +5474,10 @@
     </row>
     <row r="261" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A261" s="12" t="s">
+        <v>510</v>
+      </c>
+      <c r="B261" s="12" t="s">
         <v>511</v>
-      </c>
-      <c r="B261" s="12" t="s">
-        <v>512</v>
       </c>
       <c r="E261" s="12" t="s">
         <v>152</v>
@@ -5488,10 +5485,10 @@
     </row>
     <row r="262" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A262" s="12" t="s">
+        <v>512</v>
+      </c>
+      <c r="B262" s="12" t="s">
         <v>513</v>
-      </c>
-      <c r="B262" s="12" t="s">
-        <v>514</v>
       </c>
       <c r="E262" s="12" t="s">
         <v>152</v>
@@ -5499,10 +5496,10 @@
     </row>
     <row r="263" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A263" s="12" t="s">
+        <v>514</v>
+      </c>
+      <c r="B263" s="12" t="s">
         <v>515</v>
-      </c>
-      <c r="B263" s="12" t="s">
-        <v>516</v>
       </c>
       <c r="E263" s="12" t="s">
         <v>152</v>
@@ -5510,10 +5507,10 @@
     </row>
     <row r="264" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A264" s="12" t="s">
+        <v>516</v>
+      </c>
+      <c r="B264" s="12" t="s">
         <v>517</v>
-      </c>
-      <c r="B264" s="12" t="s">
-        <v>518</v>
       </c>
       <c r="E264" s="12" t="s">
         <v>154</v>
@@ -5521,10 +5518,10 @@
     </row>
     <row r="265" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A265" s="12" t="s">
+        <v>518</v>
+      </c>
+      <c r="B265" s="12" t="s">
         <v>519</v>
-      </c>
-      <c r="B265" s="12" t="s">
-        <v>520</v>
       </c>
       <c r="E265" s="12" t="s">
         <v>154</v>
@@ -5532,10 +5529,10 @@
     </row>
     <row r="266" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A266" s="12" t="s">
+        <v>520</v>
+      </c>
+      <c r="B266" s="12" t="s">
         <v>521</v>
-      </c>
-      <c r="B266" s="12" t="s">
-        <v>522</v>
       </c>
       <c r="E266" s="12" t="s">
         <v>154</v>
@@ -5543,10 +5540,10 @@
     </row>
     <row r="267" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A267" s="12" t="s">
+        <v>522</v>
+      </c>
+      <c r="B267" s="12" t="s">
         <v>523</v>
-      </c>
-      <c r="B267" s="12" t="s">
-        <v>524</v>
       </c>
       <c r="E267" s="12" t="s">
         <v>154</v>
@@ -5554,10 +5551,10 @@
     </row>
     <row r="268" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A268" s="12" t="s">
+        <v>524</v>
+      </c>
+      <c r="B268" s="12" t="s">
         <v>525</v>
-      </c>
-      <c r="B268" s="12" t="s">
-        <v>526</v>
       </c>
       <c r="E268" s="12" t="s">
         <v>154</v>
@@ -5565,10 +5562,10 @@
     </row>
     <row r="269" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A269" s="12" t="s">
+        <v>526</v>
+      </c>
+      <c r="B269" s="12" t="s">
         <v>527</v>
-      </c>
-      <c r="B269" s="12" t="s">
-        <v>528</v>
       </c>
       <c r="E269" s="12" t="s">
         <v>154</v>
@@ -5576,10 +5573,10 @@
     </row>
     <row r="270" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A270" s="12" t="s">
+        <v>528</v>
+      </c>
+      <c r="B270" s="12" t="s">
         <v>529</v>
-      </c>
-      <c r="B270" s="12" t="s">
-        <v>530</v>
       </c>
       <c r="E270" s="12" t="s">
         <v>156</v>
@@ -5587,10 +5584,10 @@
     </row>
     <row r="271" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A271" s="12" t="s">
+        <v>530</v>
+      </c>
+      <c r="B271" s="12" t="s">
         <v>531</v>
-      </c>
-      <c r="B271" s="12" t="s">
-        <v>532</v>
       </c>
       <c r="E271" s="12" t="s">
         <v>156</v>
@@ -5598,10 +5595,10 @@
     </row>
     <row r="272" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A272" s="12" t="s">
+        <v>532</v>
+      </c>
+      <c r="B272" s="12" t="s">
         <v>533</v>
-      </c>
-      <c r="B272" s="12" t="s">
-        <v>534</v>
       </c>
       <c r="E272" s="12" t="s">
         <v>158</v>
@@ -5609,10 +5606,10 @@
     </row>
     <row r="273" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A273" s="12" t="s">
+        <v>534</v>
+      </c>
+      <c r="B273" s="12" t="s">
         <v>535</v>
-      </c>
-      <c r="B273" s="12" t="s">
-        <v>536</v>
       </c>
       <c r="E273" s="12" t="s">
         <v>158</v>
@@ -5620,10 +5617,10 @@
     </row>
     <row r="274" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A274" s="12" t="s">
+        <v>536</v>
+      </c>
+      <c r="B274" s="12" t="s">
         <v>537</v>
-      </c>
-      <c r="B274" s="12" t="s">
-        <v>538</v>
       </c>
       <c r="E274" s="12" t="s">
         <v>158</v>
@@ -5631,10 +5628,10 @@
     </row>
     <row r="275" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A275" s="12" t="s">
+        <v>538</v>
+      </c>
+      <c r="B275" s="12" t="s">
         <v>539</v>
-      </c>
-      <c r="B275" s="12" t="s">
-        <v>540</v>
       </c>
       <c r="E275" s="12" t="s">
         <v>158</v>
@@ -5642,10 +5639,10 @@
     </row>
     <row r="276" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A276" s="12" t="s">
+        <v>540</v>
+      </c>
+      <c r="B276" s="12" t="s">
         <v>541</v>
-      </c>
-      <c r="B276" s="12" t="s">
-        <v>542</v>
       </c>
       <c r="E276" s="12" t="s">
         <v>158</v>
@@ -5653,10 +5650,10 @@
     </row>
     <row r="277" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A277" s="12" t="s">
+        <v>542</v>
+      </c>
+      <c r="B277" s="12" t="s">
         <v>543</v>
-      </c>
-      <c r="B277" s="12" t="s">
-        <v>544</v>
       </c>
       <c r="E277" s="12" t="s">
         <v>158</v>
@@ -5664,7 +5661,7 @@
     </row>
     <row r="278" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A278" s="12" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B278" s="12" t="s">
         <v>272</v>
@@ -5675,7 +5672,7 @@
     </row>
     <row r="279" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A279" s="12" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B279" s="12" t="s">
         <v>247</v>
@@ -5686,10 +5683,10 @@
     </row>
     <row r="280" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A280" s="12" t="s">
+        <v>546</v>
+      </c>
+      <c r="B280" s="12" t="s">
         <v>547</v>
-      </c>
-      <c r="B280" s="12" t="s">
-        <v>548</v>
       </c>
       <c r="E280" s="12" t="s">
         <v>160</v>
@@ -5697,7 +5694,7 @@
     </row>
     <row r="281" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A281" s="12" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B281" s="12" t="s">
         <v>295</v>
@@ -5708,7 +5705,7 @@
     </row>
     <row r="282" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A282" s="12" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B282" s="12" t="s">
         <v>263</v>
@@ -5719,10 +5716,10 @@
     </row>
     <row r="283" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A283" s="12" t="s">
+        <v>550</v>
+      </c>
+      <c r="B283" s="12" t="s">
         <v>551</v>
-      </c>
-      <c r="B283" s="12" t="s">
-        <v>552</v>
       </c>
       <c r="E283" s="12" t="s">
         <v>162</v>
@@ -5730,10 +5727,10 @@
     </row>
     <row r="284" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A284" s="12" t="s">
+        <v>552</v>
+      </c>
+      <c r="B284" s="12" t="s">
         <v>553</v>
-      </c>
-      <c r="B284" s="12" t="s">
-        <v>554</v>
       </c>
       <c r="E284" s="12" t="s">
         <v>162</v>
@@ -5741,10 +5738,10 @@
     </row>
     <row r="285" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A285" s="12" t="s">
+        <v>554</v>
+      </c>
+      <c r="B285" s="12" t="s">
         <v>555</v>
-      </c>
-      <c r="B285" s="12" t="s">
-        <v>556</v>
       </c>
       <c r="E285" s="12" t="s">
         <v>162</v>
@@ -5752,10 +5749,10 @@
     </row>
     <row r="286" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A286" s="12" t="s">
+        <v>556</v>
+      </c>
+      <c r="B286" s="12" t="s">
         <v>557</v>
-      </c>
-      <c r="B286" s="12" t="s">
-        <v>558</v>
       </c>
       <c r="E286" s="12" t="s">
         <v>162</v>
@@ -5763,10 +5760,10 @@
     </row>
     <row r="287" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A287" s="12" t="s">
+        <v>558</v>
+      </c>
+      <c r="B287" s="12" t="s">
         <v>559</v>
-      </c>
-      <c r="B287" s="12" t="s">
-        <v>560</v>
       </c>
       <c r="E287" s="12" t="s">
         <v>162</v>
@@ -5774,10 +5771,10 @@
     </row>
     <row r="288" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A288" s="12" t="s">
+        <v>560</v>
+      </c>
+      <c r="B288" s="12" t="s">
         <v>561</v>
-      </c>
-      <c r="B288" s="12" t="s">
-        <v>562</v>
       </c>
       <c r="E288" s="12" t="s">
         <v>162</v>
@@ -5785,10 +5782,10 @@
     </row>
     <row r="289" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A289" s="12" t="s">
+        <v>562</v>
+      </c>
+      <c r="B289" s="12" t="s">
         <v>563</v>
-      </c>
-      <c r="B289" s="12" t="s">
-        <v>564</v>
       </c>
       <c r="E289" s="12" t="s">
         <v>162</v>
@@ -5796,10 +5793,10 @@
     </row>
     <row r="290" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A290" s="12" t="s">
+        <v>564</v>
+      </c>
+      <c r="B290" s="12" t="s">
         <v>565</v>
-      </c>
-      <c r="B290" s="12" t="s">
-        <v>566</v>
       </c>
       <c r="E290" s="12" t="s">
         <v>162</v>
@@ -5807,7 +5804,7 @@
     </row>
     <row r="291" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A291" s="12" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B291" s="12" t="s">
         <v>247</v>
@@ -5818,10 +5815,10 @@
     </row>
     <row r="292" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A292" s="12" t="s">
+        <v>567</v>
+      </c>
+      <c r="B292" s="12" t="s">
         <v>568</v>
-      </c>
-      <c r="B292" s="12" t="s">
-        <v>569</v>
       </c>
       <c r="E292" s="12" t="s">
         <v>170</v>
@@ -5829,10 +5826,10 @@
     </row>
     <row r="293" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A293" s="12" t="s">
+        <v>569</v>
+      </c>
+      <c r="B293" s="12" t="s">
         <v>570</v>
-      </c>
-      <c r="B293" s="12" t="s">
-        <v>571</v>
       </c>
       <c r="E293" s="12" t="s">
         <v>170</v>
@@ -5840,10 +5837,10 @@
     </row>
     <row r="294" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A294" s="12" t="s">
+        <v>571</v>
+      </c>
+      <c r="B294" s="12" t="s">
         <v>572</v>
-      </c>
-      <c r="B294" s="12" t="s">
-        <v>573</v>
       </c>
       <c r="E294" s="12" t="s">
         <v>172</v>
@@ -5851,10 +5848,10 @@
     </row>
     <row r="295" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A295" s="12" t="s">
+        <v>573</v>
+      </c>
+      <c r="B295" s="12" t="s">
         <v>574</v>
-      </c>
-      <c r="B295" s="12" t="s">
-        <v>575</v>
       </c>
       <c r="E295" s="12" t="s">
         <v>172</v>
@@ -5862,10 +5859,10 @@
     </row>
     <row r="296" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A296" s="12" t="s">
+        <v>575</v>
+      </c>
+      <c r="B296" s="12" t="s">
         <v>576</v>
-      </c>
-      <c r="B296" s="12" t="s">
-        <v>577</v>
       </c>
       <c r="E296" s="12" t="s">
         <v>174</v>
@@ -5873,10 +5870,10 @@
     </row>
     <row r="297" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A297" s="12" t="s">
+        <v>577</v>
+      </c>
+      <c r="B297" s="12" t="s">
         <v>578</v>
-      </c>
-      <c r="B297" s="12" t="s">
-        <v>579</v>
       </c>
       <c r="E297" s="12" t="s">
         <v>174</v>
@@ -5884,10 +5881,10 @@
     </row>
     <row r="298" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A298" s="12" t="s">
+        <v>579</v>
+      </c>
+      <c r="B298" s="12" t="s">
         <v>580</v>
-      </c>
-      <c r="B298" s="12" t="s">
-        <v>581</v>
       </c>
       <c r="E298" s="12" t="s">
         <v>174</v>
@@ -5895,10 +5892,10 @@
     </row>
     <row r="299" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A299" s="12" t="s">
+        <v>581</v>
+      </c>
+      <c r="B299" s="12" t="s">
         <v>582</v>
-      </c>
-      <c r="B299" s="12" t="s">
-        <v>583</v>
       </c>
       <c r="E299" s="12" t="s">
         <v>174</v>
@@ -5906,10 +5903,10 @@
     </row>
     <row r="300" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A300" s="12" t="s">
+        <v>583</v>
+      </c>
+      <c r="B300" s="12" t="s">
         <v>584</v>
-      </c>
-      <c r="B300" s="12" t="s">
-        <v>585</v>
       </c>
       <c r="E300" s="12" t="s">
         <v>174</v>
@@ -5917,10 +5914,10 @@
     </row>
     <row r="301" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A301" s="12" t="s">
+        <v>585</v>
+      </c>
+      <c r="B301" s="12" t="s">
         <v>586</v>
-      </c>
-      <c r="B301" s="12" t="s">
-        <v>587</v>
       </c>
       <c r="E301" s="12" t="s">
         <v>174</v>
@@ -5928,10 +5925,10 @@
     </row>
     <row r="302" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A302" s="12" t="s">
+        <v>587</v>
+      </c>
+      <c r="B302" s="12" t="s">
         <v>588</v>
-      </c>
-      <c r="B302" s="12" t="s">
-        <v>589</v>
       </c>
       <c r="E302" s="12" t="s">
         <v>174</v>
@@ -5939,10 +5936,10 @@
     </row>
     <row r="303" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A303" s="12" t="s">
+        <v>589</v>
+      </c>
+      <c r="B303" s="12" t="s">
         <v>590</v>
-      </c>
-      <c r="B303" s="12" t="s">
-        <v>591</v>
       </c>
       <c r="E303" s="12" t="s">
         <v>176</v>
@@ -5950,10 +5947,10 @@
     </row>
     <row r="304" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A304" s="12" t="s">
+        <v>591</v>
+      </c>
+      <c r="B304" s="12" t="s">
         <v>592</v>
-      </c>
-      <c r="B304" s="12" t="s">
-        <v>593</v>
       </c>
       <c r="E304" s="12" t="s">
         <v>176</v>
@@ -5961,10 +5958,10 @@
     </row>
     <row r="305" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A305" s="12" t="s">
+        <v>593</v>
+      </c>
+      <c r="B305" s="12" t="s">
         <v>594</v>
-      </c>
-      <c r="B305" s="12" t="s">
-        <v>595</v>
       </c>
       <c r="E305" s="12" t="s">
         <v>178</v>
@@ -5972,10 +5969,10 @@
     </row>
     <row r="306" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A306" s="12" t="s">
+        <v>595</v>
+      </c>
+      <c r="B306" s="12" t="s">
         <v>596</v>
-      </c>
-      <c r="B306" s="12" t="s">
-        <v>597</v>
       </c>
       <c r="E306" s="12" t="s">
         <v>178</v>
@@ -5983,10 +5980,10 @@
     </row>
     <row r="307" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A307" s="12" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B307" s="12" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E307" s="12" t="s">
         <v>180</v>
@@ -5994,10 +5991,10 @@
     </row>
     <row r="308" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A308" s="12" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B308" s="12" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="E308" s="12" t="s">
         <v>180</v>
@@ -6005,10 +6002,10 @@
     </row>
     <row r="309" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A309" s="12" t="s">
+        <v>599</v>
+      </c>
+      <c r="B309" s="12" t="s">
         <v>600</v>
-      </c>
-      <c r="B309" s="12" t="s">
-        <v>601</v>
       </c>
       <c r="E309" s="12" t="s">
         <v>182</v>
@@ -6016,10 +6013,10 @@
     </row>
     <row r="310" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A310" s="12" t="s">
+        <v>601</v>
+      </c>
+      <c r="B310" s="12" t="s">
         <v>602</v>
-      </c>
-      <c r="B310" s="12" t="s">
-        <v>603</v>
       </c>
       <c r="E310" s="12" t="s">
         <v>182</v>
@@ -6027,10 +6024,10 @@
     </row>
     <row r="311" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A311" s="12" t="s">
+        <v>603</v>
+      </c>
+      <c r="B311" s="12" t="s">
         <v>604</v>
-      </c>
-      <c r="B311" s="12" t="s">
-        <v>605</v>
       </c>
       <c r="E311" s="12" t="s">
         <v>182</v>
@@ -6038,10 +6035,10 @@
     </row>
     <row r="312" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A312" s="12" t="s">
+        <v>605</v>
+      </c>
+      <c r="B312" s="12" t="s">
         <v>606</v>
-      </c>
-      <c r="B312" s="12" t="s">
-        <v>607</v>
       </c>
       <c r="E312" s="12" t="s">
         <v>182</v>
@@ -6049,10 +6046,10 @@
     </row>
     <row r="313" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A313" s="12" t="s">
+        <v>607</v>
+      </c>
+      <c r="B313" s="12" t="s">
         <v>608</v>
-      </c>
-      <c r="B313" s="12" t="s">
-        <v>609</v>
       </c>
       <c r="E313" s="12" t="s">
         <v>184</v>
@@ -6060,10 +6057,10 @@
     </row>
     <row r="314" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A314" s="12" t="s">
+        <v>609</v>
+      </c>
+      <c r="B314" s="12" t="s">
         <v>610</v>
-      </c>
-      <c r="B314" s="12" t="s">
-        <v>611</v>
       </c>
       <c r="E314" s="12" t="s">
         <v>184</v>
@@ -6071,10 +6068,10 @@
     </row>
     <row r="315" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A315" s="12" t="s">
+        <v>611</v>
+      </c>
+      <c r="B315" s="12" t="s">
         <v>612</v>
-      </c>
-      <c r="B315" s="12" t="s">
-        <v>613</v>
       </c>
       <c r="E315" s="12" t="s">
         <v>184</v>
@@ -6082,10 +6079,10 @@
     </row>
     <row r="316" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A316" s="12" t="s">
+        <v>613</v>
+      </c>
+      <c r="B316" s="12" t="s">
         <v>614</v>
-      </c>
-      <c r="B316" s="12" t="s">
-        <v>615</v>
       </c>
       <c r="E316" s="12" t="s">
         <v>184</v>
@@ -6093,10 +6090,10 @@
     </row>
     <row r="317" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A317" s="12" t="s">
+        <v>615</v>
+      </c>
+      <c r="B317" s="12" t="s">
         <v>616</v>
-      </c>
-      <c r="B317" s="12" t="s">
-        <v>617</v>
       </c>
       <c r="E317" s="12" t="s">
         <v>184</v>
@@ -6104,10 +6101,10 @@
     </row>
     <row r="318" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A318" s="12" t="s">
+        <v>617</v>
+      </c>
+      <c r="B318" s="12" t="s">
         <v>618</v>
-      </c>
-      <c r="B318" s="12" t="s">
-        <v>619</v>
       </c>
       <c r="E318" s="12" t="s">
         <v>186</v>
@@ -6115,10 +6112,10 @@
     </row>
     <row r="319" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A319" s="12" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B319" s="12" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E319" s="12" t="s">
         <v>186</v>
@@ -6126,10 +6123,10 @@
     </row>
     <row r="320" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A320" s="12" t="s">
+        <v>620</v>
+      </c>
+      <c r="B320" s="12" t="s">
         <v>621</v>
-      </c>
-      <c r="B320" s="12" t="s">
-        <v>622</v>
       </c>
       <c r="E320" s="12" t="s">
         <v>216</v>
@@ -6137,10 +6134,10 @@
     </row>
     <row r="321" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A321" s="12" t="s">
+        <v>622</v>
+      </c>
+      <c r="B321" s="12" t="s">
         <v>623</v>
-      </c>
-      <c r="B321" s="12" t="s">
-        <v>624</v>
       </c>
       <c r="E321" s="12" t="s">
         <v>216</v>
@@ -6148,10 +6145,10 @@
     </row>
     <row r="322" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A322" s="12" t="s">
+        <v>624</v>
+      </c>
+      <c r="B322" s="12" t="s">
         <v>625</v>
-      </c>
-      <c r="B322" s="12" t="s">
-        <v>626</v>
       </c>
       <c r="E322" s="12" t="s">
         <v>216</v>
@@ -6159,10 +6156,10 @@
     </row>
     <row r="323" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A323" s="12" t="s">
+        <v>626</v>
+      </c>
+      <c r="B323" s="12" t="s">
         <v>627</v>
-      </c>
-      <c r="B323" s="12" t="s">
-        <v>628</v>
       </c>
       <c r="E323" s="12" t="s">
         <v>216</v>
@@ -6170,10 +6167,10 @@
     </row>
     <row r="324" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A324" s="12" t="s">
+        <v>628</v>
+      </c>
+      <c r="B324" s="12" t="s">
         <v>629</v>
-      </c>
-      <c r="B324" s="12" t="s">
-        <v>630</v>
       </c>
       <c r="E324" s="12" t="s">
         <v>216</v>
@@ -6181,7 +6178,7 @@
     </row>
     <row r="325" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A325" s="12" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B325" s="12" t="s">
         <v>272</v>
@@ -6192,10 +6189,10 @@
     </row>
     <row r="326" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A326" s="12" t="s">
+        <v>631</v>
+      </c>
+      <c r="B326" s="12" t="s">
         <v>632</v>
-      </c>
-      <c r="B326" s="12" t="s">
-        <v>633</v>
       </c>
       <c r="E326" s="12" t="s">
         <v>218</v>
@@ -6203,10 +6200,10 @@
     </row>
     <row r="327" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A327" s="12" t="s">
+        <v>633</v>
+      </c>
+      <c r="B327" s="12" t="s">
         <v>634</v>
-      </c>
-      <c r="B327" s="12" t="s">
-        <v>635</v>
       </c>
       <c r="E327" s="12" t="s">
         <v>218</v>
@@ -6214,10 +6211,10 @@
     </row>
     <row r="328" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A328" s="12" t="s">
+        <v>635</v>
+      </c>
+      <c r="B328" s="12" t="s">
         <v>636</v>
-      </c>
-      <c r="B328" s="12" t="s">
-        <v>637</v>
       </c>
       <c r="E328" s="12" t="s">
         <v>218</v>
@@ -6225,10 +6222,10 @@
     </row>
     <row r="329" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A329" s="12" t="s">
+        <v>637</v>
+      </c>
+      <c r="B329" s="12" t="s">
         <v>638</v>
-      </c>
-      <c r="B329" s="12" t="s">
-        <v>639</v>
       </c>
       <c r="E329" s="12" t="s">
         <v>218</v>
@@ -6236,10 +6233,10 @@
     </row>
     <row r="330" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A330" s="12" t="s">
+        <v>639</v>
+      </c>
+      <c r="B330" s="12" t="s">
         <v>640</v>
-      </c>
-      <c r="B330" s="12" t="s">
-        <v>641</v>
       </c>
       <c r="E330" s="12" t="s">
         <v>218</v>
@@ -6247,10 +6244,10 @@
     </row>
     <row r="331" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A331" s="12" t="s">
+        <v>641</v>
+      </c>
+      <c r="B331" s="12" t="s">
         <v>642</v>
-      </c>
-      <c r="B331" s="12" t="s">
-        <v>643</v>
       </c>
       <c r="E331" s="12" t="s">
         <v>218</v>
@@ -6258,10 +6255,10 @@
     </row>
     <row r="332" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A332" s="12" t="s">
+        <v>643</v>
+      </c>
+      <c r="B332" s="12" t="s">
         <v>644</v>
-      </c>
-      <c r="B332" s="12" t="s">
-        <v>645</v>
       </c>
       <c r="E332" s="12" t="s">
         <v>220</v>
@@ -6269,10 +6266,10 @@
     </row>
     <row r="333" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A333" s="12" t="s">
+        <v>645</v>
+      </c>
+      <c r="B333" s="12" t="s">
         <v>646</v>
-      </c>
-      <c r="B333" s="12" t="s">
-        <v>647</v>
       </c>
       <c r="E333" s="12" t="s">
         <v>220</v>
@@ -6280,10 +6277,10 @@
     </row>
     <row r="334" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A334" s="12" t="s">
+        <v>647</v>
+      </c>
+      <c r="B334" s="12" t="s">
         <v>648</v>
-      </c>
-      <c r="B334" s="12" t="s">
-        <v>649</v>
       </c>
       <c r="E334" s="12" t="s">
         <v>220</v>
@@ -6291,10 +6288,10 @@
     </row>
     <row r="335" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A335" s="12" t="s">
+        <v>649</v>
+      </c>
+      <c r="B335" s="12" t="s">
         <v>650</v>
-      </c>
-      <c r="B335" s="12" t="s">
-        <v>651</v>
       </c>
       <c r="E335" s="12" t="s">
         <v>222</v>
@@ -6302,10 +6299,10 @@
     </row>
     <row r="336" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A336" s="12" t="s">
+        <v>651</v>
+      </c>
+      <c r="B336" s="12" t="s">
         <v>652</v>
-      </c>
-      <c r="B336" s="12" t="s">
-        <v>653</v>
       </c>
       <c r="E336" s="12" t="s">
         <v>222</v>
@@ -6313,10 +6310,10 @@
     </row>
     <row r="337" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A337" s="12" t="s">
+        <v>653</v>
+      </c>
+      <c r="B337" s="12" t="s">
         <v>654</v>
-      </c>
-      <c r="B337" s="12" t="s">
-        <v>655</v>
       </c>
       <c r="E337" s="12" t="s">
         <v>224</v>
@@ -6324,10 +6321,10 @@
     </row>
     <row r="338" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A338" s="12" t="s">
+        <v>655</v>
+      </c>
+      <c r="B338" s="12" t="s">
         <v>656</v>
-      </c>
-      <c r="B338" s="12" t="s">
-        <v>657</v>
       </c>
       <c r="E338" s="12" t="s">
         <v>224</v>
@@ -6335,10 +6332,10 @@
     </row>
     <row r="339" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A339" s="12" t="s">
+        <v>657</v>
+      </c>
+      <c r="B339" s="12" t="s">
         <v>658</v>
-      </c>
-      <c r="B339" s="12" t="s">
-        <v>659</v>
       </c>
       <c r="E339" s="12" t="s">
         <v>224</v>
@@ -6346,10 +6343,10 @@
     </row>
     <row r="340" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A340" s="12" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B340" s="12" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="E340" s="12" t="s">
         <v>226</v>
@@ -6357,10 +6354,10 @@
     </row>
     <row r="341" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A341" s="12" t="s">
+        <v>660</v>
+      </c>
+      <c r="B341" s="12" t="s">
         <v>661</v>
-      </c>
-      <c r="B341" s="12" t="s">
-        <v>662</v>
       </c>
       <c r="E341" s="12" t="s">
         <v>226</v>
@@ -6368,10 +6365,10 @@
     </row>
     <row r="342" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A342" s="12" t="s">
+        <v>662</v>
+      </c>
+      <c r="B342" s="12" t="s">
         <v>663</v>
-      </c>
-      <c r="B342" s="12" t="s">
-        <v>664</v>
       </c>
       <c r="E342" s="12" t="s">
         <v>226</v>
@@ -6379,10 +6376,10 @@
     </row>
     <row r="343" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A343" s="12" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B343" s="12" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E343" s="12" t="s">
         <v>226</v>
@@ -6390,10 +6387,10 @@
     </row>
     <row r="344" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A344" s="12" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B344" s="12" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="E344" s="12" t="s">
         <v>228</v>
@@ -6401,10 +6398,10 @@
     </row>
     <row r="345" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A345" s="12" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B345" s="12" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="E345" s="12" t="s">
         <v>228</v>
@@ -6412,10 +6409,10 @@
     </row>
     <row r="346" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A346" s="12" t="s">
+        <v>667</v>
+      </c>
+      <c r="B346" s="12" t="s">
         <v>668</v>
-      </c>
-      <c r="B346" s="12" t="s">
-        <v>669</v>
       </c>
       <c r="E346" s="12" t="s">
         <v>228</v>
@@ -6423,10 +6420,10 @@
     </row>
     <row r="347" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A347" s="12" t="s">
+        <v>669</v>
+      </c>
+      <c r="B347" s="12" t="s">
         <v>670</v>
-      </c>
-      <c r="B347" s="12" t="s">
-        <v>671</v>
       </c>
       <c r="E347" s="12" t="s">
         <v>230</v>
@@ -6434,10 +6431,10 @@
     </row>
     <row r="348" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A348" s="12" t="s">
+        <v>671</v>
+      </c>
+      <c r="B348" s="12" t="s">
         <v>672</v>
-      </c>
-      <c r="B348" s="12" t="s">
-        <v>673</v>
       </c>
       <c r="E348" s="12" t="s">
         <v>230</v>
@@ -6445,10 +6442,10 @@
     </row>
     <row r="349" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A349" s="12" t="s">
+        <v>673</v>
+      </c>
+      <c r="B349" s="12" t="s">
         <v>674</v>
-      </c>
-      <c r="B349" s="12" t="s">
-        <v>675</v>
       </c>
       <c r="E349" s="12" t="s">
         <v>230</v>
@@ -6456,10 +6453,10 @@
     </row>
     <row r="350" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A350" s="12" t="s">
+        <v>675</v>
+      </c>
+      <c r="B350" s="12" t="s">
         <v>676</v>
-      </c>
-      <c r="B350" s="12" t="s">
-        <v>677</v>
       </c>
       <c r="E350" s="12" t="s">
         <v>96</v>
@@ -6467,10 +6464,10 @@
     </row>
     <row r="351" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A351" s="12" t="s">
+        <v>677</v>
+      </c>
+      <c r="B351" s="12" t="s">
         <v>678</v>
-      </c>
-      <c r="B351" s="12" t="s">
-        <v>679</v>
       </c>
       <c r="E351" s="12" t="s">
         <v>96</v>
@@ -6478,10 +6475,10 @@
     </row>
     <row r="352" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A352" s="12" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B352" s="12" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="E352" s="12" t="s">
         <v>96</v>
@@ -6489,10 +6486,10 @@
     </row>
     <row r="353" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A353" s="12" t="s">
+        <v>680</v>
+      </c>
+      <c r="B353" s="12" t="s">
         <v>681</v>
-      </c>
-      <c r="B353" s="12" t="s">
-        <v>682</v>
       </c>
       <c r="E353" s="12" t="s">
         <v>96</v>
@@ -6500,10 +6497,10 @@
     </row>
     <row r="354" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A354" s="12" t="s">
+        <v>682</v>
+      </c>
+      <c r="B354" s="12" t="s">
         <v>683</v>
-      </c>
-      <c r="B354" s="12" t="s">
-        <v>684</v>
       </c>
       <c r="E354" s="12" t="s">
         <v>96</v>

</xml_diff>

<commit_message>
ENH:Use same labels as the original taxonomy
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="684">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1068" uniqueCount="682">
   <si>
     <t xml:space="preserve">ConceptScheme URI</t>
   </si>
@@ -208,6 +208,9 @@
     <t xml:space="preserve">Meterological Station</t>
   </si>
   <si>
+    <t xml:space="preserve">"Reliawind Taxonomy ambiguously classifies this concept as a Sub-System, an Assembly, a Sub-assembly, and a Component."</t>
+  </si>
+  <si>
     <t xml:space="preserve">reliatax:OperationalInfrastructure</t>
   </si>
   <si>
@@ -316,10 +319,16 @@
     <t xml:space="preserve">Tower</t>
   </si>
   <si>
+    <t xml:space="preserve">"Reliawind Taxonomy ambiguously classifies this concept both as an Assembly and a Sub-assembly."</t>
+  </si>
+  <si>
     <t xml:space="preserve">reliatax:CollectionSystemCable</t>
   </si>
   <si>
-    <t xml:space="preserve">Collection System Cable</t>
+    <t xml:space="preserve">Cable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Reliawind Taxonomy ambiguously classifies this concept as an Assembly, a Sub-assembly, and a Component."</t>
   </si>
   <si>
     <t xml:space="preserve">reliatax:GridConnection</t>
@@ -337,7 +346,7 @@
     <t xml:space="preserve">reliatax:GearboxCoolingSystem</t>
   </si>
   <si>
-    <t xml:space="preserve">Gearbox Cooling System</t>
+    <t xml:space="preserve">Cooling System</t>
   </si>
   <si>
     <t xml:space="preserve">reliatax:GearboxGears</t>
@@ -355,49 +364,40 @@
     <t xml:space="preserve">reliatax:GearboxLubricationSystem</t>
   </si>
   <si>
-    <t xml:space="preserve">Gearbox Lubrication System</t>
+    <t xml:space="preserve">Lubrication System</t>
   </si>
   <si>
     <t xml:space="preserve">reliatax:GearboxSensors</t>
   </si>
   <si>
-    <t xml:space="preserve">Gearbox Sensors</t>
+    <t xml:space="preserve">Sensors</t>
   </si>
   <si>
     <t xml:space="preserve">reliatax:GeneratorCoolingSystem</t>
   </si>
   <si>
-    <t xml:space="preserve">Generator Cooling System</t>
-  </si>
-  <si>
     <t xml:space="preserve">reliatax:GeneratorLubricationSystem</t>
   </si>
   <si>
-    <t xml:space="preserve">Generator Lubrication System</t>
-  </si>
-  <si>
     <t xml:space="preserve">reliatax:GeneratorSensors</t>
   </si>
   <si>
-    <t xml:space="preserve">Generator Sensors</t>
-  </si>
-  <si>
     <t xml:space="preserve">reliatax:GeneratorRotor</t>
   </si>
   <si>
-    <t xml:space="preserve">Generator Rotor</t>
+    <t xml:space="preserve">Rotor</t>
   </si>
   <si>
     <t xml:space="preserve">reliatax:GeneratorStator</t>
   </si>
   <si>
-    <t xml:space="preserve">Generator Stator</t>
+    <t xml:space="preserve">Stator</t>
   </si>
   <si>
     <t xml:space="preserve">reliatax:GeneratorStructuralMechanical</t>
   </si>
   <si>
-    <t xml:space="preserve">Generator Structural and Mechanical</t>
+    <t xml:space="preserve">Structural &amp; Mechanical</t>
   </si>
   <si>
     <t xml:space="preserve">reliatax:HighSpeedSide</t>
@@ -421,9 +421,6 @@
     <t xml:space="preserve">reliatax:MainShaftSetSensors</t>
   </si>
   <si>
-    <t xml:space="preserve">Main ShaftSet Sensors</t>
-  </si>
-  <si>
     <t xml:space="preserve">reliatax:ElectricalServices</t>
   </si>
   <si>
@@ -592,6 +589,9 @@
     <t xml:space="preserve">Blade Lightning Protection Termination</t>
   </si>
   <si>
+    <t xml:space="preserve">"Reliawind Taxonomy classifies this concept both as a Sub-assembly and as a Component."</t>
+  </si>
+  <si>
     <t xml:space="preserve">reliatax:BladeLightningDownConductor</t>
   </si>
   <si>
@@ -1285,9 +1285,6 @@
     <t xml:space="preserve">reliatax:ControlAndCommunicationSystemAncillaryEquipmentCable</t>
   </si>
   <si>
-    <t xml:space="preserve">Cable</t>
-  </si>
-  <si>
     <t xml:space="preserve">reliatax:ControlAndCommunicationSystemAncillaryEquipmentContactor</t>
   </si>
   <si>
@@ -1349,9 +1346,6 @@
   </si>
   <si>
     <t xml:space="preserve">reliatax:ControlAndCommunicationSystemConditionMonitoringSystemSensor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sensors</t>
   </si>
   <si>
     <t xml:space="preserve">reliatax:ControlAndCommunicationSystemControllerHardwareControllerPowerSupply</t>
@@ -2201,7 +2195,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2271,6 +2265,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2529,8 +2531,8 @@
   </sheetPr>
   <dimension ref="A1:I359"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A207" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F206" activeCellId="0" sqref="F206"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C13" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I29" activeCellId="0" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2707,7 +2709,7 @@
         <f aca="false">IF(ISBLANK($B21),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B21," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
         <v>reliatax:WindTurbine</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="12" t="s">
         <v>35</v>
       </c>
       <c r="C21" s="12" t="s">
@@ -2720,14 +2722,14 @@
       </c>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
+      <c r="I21" s="13"/>
     </row>
     <row r="22" s="10" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="11" t="str">
         <f aca="false">IF(ISBLANK($B22),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B22," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
         <v>reliatax:WindFarm</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="12" t="s">
         <v>38</v>
       </c>
       <c r="C22" s="12" t="s">
@@ -2738,7 +2740,7 @@
       <c r="F22" s="11"/>
       <c r="G22" s="16"/>
       <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
+      <c r="I22" s="13"/>
     </row>
     <row r="23" s="10" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="12" t="s">
@@ -2757,7 +2759,7 @@
       <c r="F23" s="11"/>
       <c r="G23" s="16"/>
       <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
+      <c r="I23" s="13"/>
     </row>
     <row r="24" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="12" t="s">
@@ -2778,9 +2780,9 @@
       </c>
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-    </row>
-    <row r="25" s="10" customFormat="true" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I24" s="13"/>
+    </row>
+    <row r="25" s="10" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="12" t="s">
         <v>48</v>
       </c>
@@ -2799,7 +2801,7 @@
       <c r="F25" s="15"/>
       <c r="G25" s="16"/>
       <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
+      <c r="I25" s="13"/>
     </row>
     <row r="26" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="12" t="s">
@@ -2818,7 +2820,7 @@
       <c r="F26" s="11"/>
       <c r="G26" s="16"/>
       <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
+      <c r="I26" s="13"/>
     </row>
     <row r="27" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="12" t="s">
@@ -2835,7 +2837,7 @@
       <c r="F27" s="15"/>
       <c r="G27" s="16"/>
       <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
+      <c r="I27" s="13"/>
     </row>
     <row r="28" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="12" t="s">
@@ -2852,7 +2854,7 @@
       <c r="F28" s="11"/>
       <c r="G28" s="16"/>
       <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
+      <c r="I28" s="13"/>
     </row>
     <row r="29" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="12" t="s">
@@ -2869,14 +2871,16 @@
       <c r="F29" s="11"/>
       <c r="G29" s="16"/>
       <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
+      <c r="I29" s="18" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="30" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="12" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
@@ -2886,14 +2890,16 @@
       <c r="F30" s="11"/>
       <c r="G30" s="16"/>
       <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
+      <c r="I30" s="18" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="31" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C31" s="11"/>
       <c r="D31" s="11"/>
@@ -2903,14 +2909,14 @@
       <c r="F31" s="11"/>
       <c r="G31" s="16"/>
       <c r="H31" s="11"/>
-      <c r="I31" s="11"/>
+      <c r="I31" s="19"/>
     </row>
     <row r="32" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="11"/>
@@ -2920,14 +2926,14 @@
       <c r="F32" s="11"/>
       <c r="G32" s="16"/>
       <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
+      <c r="I32" s="19"/>
     </row>
     <row r="33" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C33" s="11"/>
       <c r="D33" s="11"/>
@@ -2937,14 +2943,14 @@
       <c r="F33" s="11"/>
       <c r="G33" s="16"/>
       <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
+      <c r="I33" s="19"/>
     </row>
     <row r="34" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C34" s="11"/>
       <c r="D34" s="11"/>
@@ -2954,14 +2960,14 @@
       <c r="F34" s="11"/>
       <c r="G34" s="16"/>
       <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
+      <c r="I34" s="19"/>
     </row>
     <row r="35" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="12" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C35" s="11"/>
       <c r="D35" s="11"/>
@@ -2971,14 +2977,14 @@
       <c r="F35" s="11"/>
       <c r="G35" s="16"/>
       <c r="H35" s="11"/>
-      <c r="I35" s="11"/>
+      <c r="I35" s="13"/>
     </row>
     <row r="36" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="12" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C36" s="11"/>
       <c r="D36" s="11"/>
@@ -2988,14 +2994,14 @@
       <c r="F36" s="11"/>
       <c r="G36" s="16"/>
       <c r="H36" s="11"/>
-      <c r="I36" s="11"/>
+      <c r="I36" s="13"/>
     </row>
     <row r="37" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C37" s="11"/>
       <c r="D37" s="11"/>
@@ -3005,31 +3011,31 @@
       <c r="F37" s="11"/>
       <c r="G37" s="16"/>
       <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
+      <c r="I37" s="13"/>
     </row>
     <row r="38" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="12" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C38" s="11"/>
       <c r="D38" s="11"/>
       <c r="E38" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="F38" s="18"/>
+      <c r="F38" s="20"/>
       <c r="G38" s="16"/>
       <c r="H38" s="11"/>
-      <c r="I38" s="11"/>
+      <c r="I38" s="13"/>
     </row>
     <row r="39" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="12" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C39" s="11"/>
       <c r="D39" s="11"/>
@@ -3039,216 +3045,239 @@
       <c r="F39" s="11"/>
       <c r="G39" s="16"/>
       <c r="H39" s="11"/>
-      <c r="I39" s="11"/>
+      <c r="I39" s="13"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E40" s="12" t="s">
         <v>48</v>
       </c>
+      <c r="I40" s="13"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="12" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E41" s="12" t="s">
         <v>48</v>
       </c>
+      <c r="I41" s="13"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="12" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E42" s="12" t="s">
         <v>48</v>
       </c>
+      <c r="I42" s="13"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E43" s="12" t="s">
         <v>52</v>
       </c>
+      <c r="I43" s="13"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="12" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E44" s="12" t="s">
         <v>52</v>
       </c>
+      <c r="I44" s="13"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="12" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E45" s="12" t="s">
         <v>52</v>
       </c>
+      <c r="I45" s="13"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="12" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E46" s="12" t="s">
         <v>55</v>
       </c>
+      <c r="I46" s="13"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="12" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E47" s="12" t="s">
         <v>55</v>
       </c>
+      <c r="I47" s="12" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="12" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E48" s="12" t="s">
         <v>57</v>
       </c>
+      <c r="I48" s="12" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="12" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>64</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="I49" s="13"/>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="12" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>66</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="I50" s="13"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="12" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>66</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="I51" s="13"/>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="12" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>66</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="I52" s="13"/>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="12" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>66</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="I53" s="13"/>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="12" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>66</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="I54" s="13"/>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="12" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>66</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="I55" s="13"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="12" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>68</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="I56" s="13"/>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="12" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>68</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="I57" s="13"/>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="12" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E58" s="12" t="s">
-        <v>68</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="I58" s="13"/>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="12" t="s">
@@ -3258,8 +3287,9 @@
         <v>121</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>68</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="I59" s="13"/>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="12" t="s">
@@ -3269,8 +3299,9 @@
         <v>123</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>68</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="I60" s="13"/>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="12" t="s">
@@ -3280,8 +3311,9 @@
         <v>125</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>68</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="I61" s="13"/>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="12" t="s">
@@ -3291,8 +3323,9 @@
         <v>127</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>70</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="I62" s="13"/>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="12" t="s">
@@ -3302,8 +3335,9 @@
         <v>129</v>
       </c>
       <c r="E63" s="12" t="s">
-        <v>70</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="I63" s="13"/>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="12" t="s">
@@ -3313,326 +3347,358 @@
         <v>131</v>
       </c>
       <c r="E64" s="12" t="s">
-        <v>70</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="I64" s="13"/>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="12" t="s">
         <v>132</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="E65" s="12" t="s">
-        <v>70</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="I65" s="13"/>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="B66" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="B66" s="12" t="s">
-        <v>135</v>
-      </c>
       <c r="E66" s="12" t="s">
-        <v>72</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="I66" s="13"/>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="B67" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="B67" s="12" t="s">
-        <v>137</v>
-      </c>
       <c r="E67" s="12" t="s">
-        <v>72</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="I67" s="13"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="B68" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="B68" s="12" t="s">
-        <v>139</v>
-      </c>
       <c r="E68" s="12" t="s">
-        <v>74</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="I68" s="13"/>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="B69" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="B69" s="12" t="s">
-        <v>141</v>
-      </c>
       <c r="E69" s="12" t="s">
-        <v>74</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="I69" s="13"/>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="B70" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="B70" s="12" t="s">
-        <v>143</v>
-      </c>
       <c r="E70" s="12" t="s">
-        <v>74</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="I70" s="13"/>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="B71" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="B71" s="12" t="s">
-        <v>145</v>
-      </c>
       <c r="E71" s="12" t="s">
-        <v>74</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="I71" s="13"/>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="B72" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="B72" s="12" t="s">
-        <v>147</v>
-      </c>
       <c r="E72" s="12" t="s">
-        <v>74</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="I72" s="13"/>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="B73" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="B73" s="12" t="s">
-        <v>149</v>
-      </c>
       <c r="E73" s="12" t="s">
-        <v>74</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="I73" s="13"/>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="B74" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="B74" s="12" t="s">
-        <v>151</v>
-      </c>
       <c r="E74" s="12" t="s">
-        <v>76</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="I74" s="13"/>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="B75" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="B75" s="12" t="s">
-        <v>153</v>
-      </c>
       <c r="E75" s="12" t="s">
-        <v>76</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="I75" s="13"/>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="B76" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="B76" s="12" t="s">
-        <v>155</v>
-      </c>
       <c r="E76" s="12" t="s">
-        <v>76</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="I76" s="13"/>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="B77" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="B77" s="12" t="s">
-        <v>157</v>
-      </c>
       <c r="E77" s="12" t="s">
-        <v>78</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="I77" s="13"/>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="B78" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="B78" s="12" t="s">
-        <v>159</v>
-      </c>
       <c r="E78" s="12" t="s">
-        <v>78</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="I78" s="13"/>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="B79" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="B79" s="12" t="s">
-        <v>161</v>
-      </c>
       <c r="E79" s="12" t="s">
-        <v>80</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="I79" s="13"/>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="B80" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="B80" s="12" t="s">
-        <v>163</v>
-      </c>
       <c r="E80" s="12" t="s">
-        <v>80</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="I80" s="13"/>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="B81" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="B81" s="12" t="s">
-        <v>165</v>
-      </c>
       <c r="E81" s="12" t="s">
-        <v>80</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="I81" s="13"/>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="B82" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="B82" s="12" t="s">
-        <v>167</v>
-      </c>
       <c r="E82" s="12" t="s">
-        <v>80</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="I82" s="13"/>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="B83" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="B83" s="12" t="s">
-        <v>169</v>
-      </c>
       <c r="E83" s="12" t="s">
-        <v>80</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="I83" s="13"/>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="B84" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="B84" s="12" t="s">
-        <v>171</v>
-      </c>
       <c r="E84" s="12" t="s">
-        <v>82</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="I84" s="13"/>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="B85" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="B85" s="12" t="s">
-        <v>173</v>
-      </c>
       <c r="E85" s="12" t="s">
-        <v>82</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="I85" s="13"/>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="B86" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="B86" s="12" t="s">
-        <v>175</v>
-      </c>
       <c r="E86" s="12" t="s">
-        <v>82</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="I86" s="13"/>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="B87" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="B87" s="12" t="s">
-        <v>177</v>
-      </c>
       <c r="E87" s="12" t="s">
-        <v>84</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="I87" s="13"/>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="B88" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="B88" s="12" t="s">
-        <v>179</v>
-      </c>
       <c r="E88" s="12" t="s">
-        <v>84</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="I88" s="13"/>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="B89" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="B89" s="12" t="s">
-        <v>181</v>
-      </c>
       <c r="E89" s="12" t="s">
-        <v>84</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="I89" s="13"/>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="B90" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="B90" s="12" t="s">
-        <v>183</v>
-      </c>
       <c r="E90" s="12" t="s">
-        <v>86</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="I90" s="13"/>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="B91" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="B91" s="12" t="s">
-        <v>185</v>
-      </c>
       <c r="E91" s="12" t="s">
-        <v>86</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="I91" s="13"/>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="B92" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="B92" s="12" t="s">
-        <v>187</v>
-      </c>
       <c r="E92" s="12" t="s">
-        <v>86</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="I92" s="13"/>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="B93" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="B93" s="12" t="s">
+      <c r="E93" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="I93" s="12" t="s">
         <v>189</v>
-      </c>
-      <c r="E93" s="12" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3643,7 +3709,10 @@
         <v>191</v>
       </c>
       <c r="E94" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
+      </c>
+      <c r="I94" s="12" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3654,7 +3723,10 @@
         <v>193</v>
       </c>
       <c r="E95" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
+      </c>
+      <c r="I95" s="12" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3665,7 +3737,10 @@
         <v>195</v>
       </c>
       <c r="E96" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
+      </c>
+      <c r="I96" s="12" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3676,7 +3751,10 @@
         <v>197</v>
       </c>
       <c r="E97" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
+      </c>
+      <c r="I97" s="12" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3687,7 +3765,10 @@
         <v>199</v>
       </c>
       <c r="E98" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
+      </c>
+      <c r="I98" s="12" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3698,7 +3779,10 @@
         <v>201</v>
       </c>
       <c r="E99" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
+      </c>
+      <c r="I99" s="12" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3709,7 +3793,10 @@
         <v>203</v>
       </c>
       <c r="E100" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
+      </c>
+      <c r="I100" s="12" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3720,7 +3807,10 @@
         <v>205</v>
       </c>
       <c r="E101" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
+      </c>
+      <c r="I101" s="12" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3731,7 +3821,10 @@
         <v>207</v>
       </c>
       <c r="E102" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
+      </c>
+      <c r="I102" s="12" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3742,7 +3835,10 @@
         <v>209</v>
       </c>
       <c r="E103" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
+      </c>
+      <c r="I103" s="12" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3753,7 +3849,10 @@
         <v>211</v>
       </c>
       <c r="E104" s="12" t="s">
-        <v>88</v>
+        <v>89</v>
+      </c>
+      <c r="I104" s="12" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3764,7 +3863,10 @@
         <v>213</v>
       </c>
       <c r="E105" s="12" t="s">
-        <v>90</v>
+        <v>91</v>
+      </c>
+      <c r="I105" s="12" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3775,7 +3877,10 @@
         <v>215</v>
       </c>
       <c r="E106" s="12" t="s">
-        <v>90</v>
+        <v>91</v>
+      </c>
+      <c r="I106" s="12" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3786,8 +3891,9 @@
         <v>217</v>
       </c>
       <c r="E107" s="12" t="s">
-        <v>92</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="I107" s="13"/>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="12" t="s">
@@ -3797,8 +3903,9 @@
         <v>219</v>
       </c>
       <c r="E108" s="12" t="s">
-        <v>92</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="I108" s="13"/>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="12" t="s">
@@ -3808,8 +3915,9 @@
         <v>221</v>
       </c>
       <c r="E109" s="12" t="s">
-        <v>92</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="I109" s="13"/>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="12" t="s">
@@ -3819,8 +3927,9 @@
         <v>223</v>
       </c>
       <c r="E110" s="12" t="s">
-        <v>94</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="I110" s="13"/>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="12" t="s">
@@ -3830,8 +3939,9 @@
         <v>225</v>
       </c>
       <c r="E111" s="12" t="s">
-        <v>94</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="I111" s="13"/>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="12" t="s">
@@ -3841,8 +3951,9 @@
         <v>227</v>
       </c>
       <c r="E112" s="12" t="s">
-        <v>94</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="I112" s="13"/>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="12" t="s">
@@ -3852,8 +3963,9 @@
         <v>229</v>
       </c>
       <c r="E113" s="12" t="s">
-        <v>94</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="I113" s="13"/>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="12" t="s">
@@ -3863,8 +3975,9 @@
         <v>231</v>
       </c>
       <c r="E114" s="12" t="s">
-        <v>96</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="I114" s="13"/>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="12" t="s">
@@ -3874,7 +3987,10 @@
         <v>233</v>
       </c>
       <c r="E115" s="12" t="s">
-        <v>100</v>
+        <v>103</v>
+      </c>
+      <c r="I115" s="12" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3885,7 +4001,10 @@
         <v>235</v>
       </c>
       <c r="E116" s="12" t="s">
-        <v>100</v>
+        <v>103</v>
+      </c>
+      <c r="I116" s="12" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3896,7 +4015,10 @@
         <v>237</v>
       </c>
       <c r="E117" s="12" t="s">
-        <v>100</v>
+        <v>103</v>
+      </c>
+      <c r="I117" s="12" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3907,8 +4029,9 @@
         <v>239</v>
       </c>
       <c r="E118" s="12" t="s">
-        <v>102</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="I118" s="13"/>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="12" t="s">
@@ -3918,8 +4041,9 @@
         <v>241</v>
       </c>
       <c r="E119" s="12" t="s">
-        <v>102</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="I119" s="13"/>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="12" t="s">
@@ -3929,8 +4053,9 @@
         <v>243</v>
       </c>
       <c r="E120" s="12" t="s">
-        <v>102</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="I120" s="13"/>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="12" t="s">
@@ -3940,7 +4065,7 @@
         <v>245</v>
       </c>
       <c r="E121" s="12" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3951,7 +4076,7 @@
         <v>247</v>
       </c>
       <c r="E122" s="12" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3962,7 +4087,7 @@
         <v>249</v>
       </c>
       <c r="E123" s="12" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3973,7 +4098,7 @@
         <v>251</v>
       </c>
       <c r="E124" s="12" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3984,7 +4109,7 @@
         <v>253</v>
       </c>
       <c r="E125" s="12" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3995,7 +4120,7 @@
         <v>255</v>
       </c>
       <c r="E126" s="12" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4006,7 +4131,7 @@
         <v>257</v>
       </c>
       <c r="E127" s="12" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4017,7 +4142,7 @@
         <v>259</v>
       </c>
       <c r="E128" s="12" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4028,7 +4153,7 @@
         <v>261</v>
       </c>
       <c r="E129" s="12" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4039,7 +4164,7 @@
         <v>263</v>
       </c>
       <c r="E130" s="12" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4050,7 +4175,7 @@
         <v>265</v>
       </c>
       <c r="E131" s="12" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4061,7 +4186,7 @@
         <v>267</v>
       </c>
       <c r="E132" s="12" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4072,7 +4197,7 @@
         <v>269</v>
       </c>
       <c r="E133" s="12" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4083,7 +4208,7 @@
         <v>245</v>
       </c>
       <c r="E134" s="12" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4094,7 +4219,7 @@
         <v>272</v>
       </c>
       <c r="E135" s="12" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4105,7 +4230,7 @@
         <v>274</v>
       </c>
       <c r="E136" s="12" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4116,7 +4241,7 @@
         <v>247</v>
       </c>
       <c r="E137" s="12" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4127,7 +4252,7 @@
         <v>277</v>
       </c>
       <c r="E138" s="12" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4138,7 +4263,7 @@
         <v>279</v>
       </c>
       <c r="E139" s="12" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4149,7 +4274,7 @@
         <v>281</v>
       </c>
       <c r="E140" s="12" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4160,7 +4285,7 @@
         <v>283</v>
       </c>
       <c r="E141" s="12" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4171,7 +4296,7 @@
         <v>285</v>
       </c>
       <c r="E142" s="12" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4182,7 +4307,7 @@
         <v>287</v>
       </c>
       <c r="E143" s="12" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4193,7 +4318,7 @@
         <v>289</v>
       </c>
       <c r="E144" s="12" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4204,7 +4329,7 @@
         <v>291</v>
       </c>
       <c r="E145" s="12" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4215,7 +4340,7 @@
         <v>293</v>
       </c>
       <c r="E146" s="12" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4226,7 +4351,7 @@
         <v>295</v>
       </c>
       <c r="E147" s="12" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4237,7 +4362,7 @@
         <v>245</v>
       </c>
       <c r="E148" s="12" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4248,7 +4373,7 @@
         <v>249</v>
       </c>
       <c r="E149" s="12" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4259,7 +4384,7 @@
         <v>247</v>
       </c>
       <c r="E150" s="12" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4270,7 +4395,7 @@
         <v>277</v>
       </c>
       <c r="E151" s="12" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4347,7 +4472,7 @@
         <v>313</v>
       </c>
       <c r="E158" s="12" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4358,7 +4483,7 @@
         <v>315</v>
       </c>
       <c r="E159" s="12" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4369,7 +4494,7 @@
         <v>317</v>
       </c>
       <c r="E160" s="12" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4421,7 +4546,7 @@
         <v>326</v>
       </c>
       <c r="B165" s="12" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E165" s="12" t="s">
         <v>124</v>
@@ -4688,7 +4813,7 @@
         <v>371</v>
       </c>
       <c r="E189" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4699,7 +4824,7 @@
         <v>373</v>
       </c>
       <c r="E190" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4710,7 +4835,7 @@
         <v>375</v>
       </c>
       <c r="E191" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4721,7 +4846,7 @@
         <v>377</v>
       </c>
       <c r="E192" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4732,7 +4857,7 @@
         <v>379</v>
       </c>
       <c r="E193" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4743,7 +4868,7 @@
         <v>381</v>
       </c>
       <c r="E194" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4754,7 +4879,7 @@
         <v>383</v>
       </c>
       <c r="E195" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4765,7 +4890,7 @@
         <v>385</v>
       </c>
       <c r="E196" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4776,7 +4901,7 @@
         <v>387</v>
       </c>
       <c r="E197" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4787,7 +4912,7 @@
         <v>389</v>
       </c>
       <c r="E198" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4798,7 +4923,7 @@
         <v>391</v>
       </c>
       <c r="E199" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4809,7 +4934,7 @@
         <v>393</v>
       </c>
       <c r="E200" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4820,7 +4945,7 @@
         <v>395</v>
       </c>
       <c r="E201" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4831,7 +4956,7 @@
         <v>397</v>
       </c>
       <c r="E202" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4842,7 +4967,7 @@
         <v>399</v>
       </c>
       <c r="E203" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4853,7 +4978,7 @@
         <v>401</v>
       </c>
       <c r="E204" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4864,7 +4989,7 @@
         <v>403</v>
       </c>
       <c r="E205" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4875,7 +5000,7 @@
         <v>405</v>
       </c>
       <c r="E206" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4886,7 +5011,7 @@
         <v>407</v>
       </c>
       <c r="E207" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4897,7 +5022,7 @@
         <v>409</v>
       </c>
       <c r="E208" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4908,7 +5033,7 @@
         <v>411</v>
       </c>
       <c r="E209" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4919,7 +5044,7 @@
         <v>413</v>
       </c>
       <c r="E210" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4930,7 +5055,7 @@
         <v>415</v>
       </c>
       <c r="E211" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4941,7 +5066,7 @@
         <v>399</v>
       </c>
       <c r="E212" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4952,7 +5077,7 @@
         <v>375</v>
       </c>
       <c r="E213" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4963,7 +5088,7 @@
         <v>419</v>
       </c>
       <c r="E214" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4971,1162 +5096,1162 @@
         <v>420</v>
       </c>
       <c r="B215" s="12" t="s">
-        <v>421</v>
+        <v>101</v>
       </c>
       <c r="E215" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A216" s="12" t="s">
+        <v>421</v>
+      </c>
+      <c r="B216" s="12" t="s">
         <v>422</v>
       </c>
-      <c r="B216" s="12" t="s">
-        <v>423</v>
-      </c>
       <c r="E216" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A217" s="12" t="s">
+        <v>423</v>
+      </c>
+      <c r="B217" s="12" t="s">
         <v>424</v>
       </c>
-      <c r="B217" s="12" t="s">
-        <v>425</v>
-      </c>
       <c r="E217" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A218" s="12" t="s">
+        <v>425</v>
+      </c>
+      <c r="B218" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="B218" s="12" t="s">
-        <v>427</v>
-      </c>
       <c r="E218" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A219" s="12" t="s">
+        <v>427</v>
+      </c>
+      <c r="B219" s="12" t="s">
         <v>428</v>
       </c>
-      <c r="B219" s="12" t="s">
-        <v>429</v>
-      </c>
       <c r="E219" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A220" s="12" t="s">
+        <v>429</v>
+      </c>
+      <c r="B220" s="12" t="s">
         <v>430</v>
       </c>
-      <c r="B220" s="12" t="s">
-        <v>431</v>
-      </c>
       <c r="E220" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A221" s="12" t="s">
+        <v>431</v>
+      </c>
+      <c r="B221" s="12" t="s">
         <v>432</v>
       </c>
-      <c r="B221" s="12" t="s">
-        <v>433</v>
-      </c>
       <c r="E221" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A222" s="12" t="s">
+        <v>433</v>
+      </c>
+      <c r="B222" s="12" t="s">
         <v>434</v>
       </c>
-      <c r="B222" s="12" t="s">
-        <v>435</v>
-      </c>
       <c r="E222" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A223" s="12" t="s">
+        <v>435</v>
+      </c>
+      <c r="B223" s="12" t="s">
         <v>436</v>
       </c>
-      <c r="B223" s="12" t="s">
-        <v>437</v>
-      </c>
       <c r="E223" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A224" s="12" t="s">
+        <v>437</v>
+      </c>
+      <c r="B224" s="12" t="s">
         <v>438</v>
       </c>
-      <c r="B224" s="12" t="s">
-        <v>439</v>
-      </c>
       <c r="E224" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A225" s="12" t="s">
+        <v>439</v>
+      </c>
+      <c r="B225" s="12" t="s">
         <v>440</v>
       </c>
-      <c r="B225" s="12" t="s">
-        <v>441</v>
-      </c>
       <c r="E225" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A226" s="12" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B226" s="12" t="s">
-        <v>443</v>
+        <v>116</v>
       </c>
       <c r="E226" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A227" s="12" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B227" s="12" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="E227" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A228" s="12" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B228" s="12" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="E228" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A229" s="12" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B229" s="12" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="E229" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A230" s="12" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B230" s="12" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="E230" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A231" s="12" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B231" s="12" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="E231" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A232" s="12" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B232" s="12" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="E232" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A233" s="12" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B233" s="12" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E233" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A234" s="12" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B234" s="12" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E234" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A235" s="12" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B235" s="12" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="E235" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A236" s="12" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B236" s="12" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="E236" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A237" s="12" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B237" s="12" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="E237" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A238" s="12" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B238" s="12" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="E238" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A239" s="12" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B239" s="12" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="E239" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A240" s="12" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B240" s="12" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="E240" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A241" s="12" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B241" s="12" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="E241" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A242" s="12" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B242" s="12" t="s">
         <v>377</v>
       </c>
       <c r="E242" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A243" s="12" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B243" s="12" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E243" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A244" s="12" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B244" s="12" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="E244" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A245" s="12" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B245" s="12" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="E245" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A246" s="12" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B246" s="12" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="E246" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A247" s="12" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B247" s="12" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="E247" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A248" s="12" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B248" s="12" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="E248" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A249" s="12" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B249" s="12" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="E249" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A250" s="12" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B250" s="12" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="E250" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A251" s="12" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B251" s="12" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="E251" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A252" s="12" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B252" s="12" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="E252" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A253" s="12" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B253" s="12" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="E253" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A254" s="12" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B254" s="12" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E254" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A255" s="12" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B255" s="12" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="E255" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A256" s="12" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B256" s="12" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E256" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A257" s="12" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B257" s="12" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="E257" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A258" s="12" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B258" s="12" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="E258" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A259" s="12" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B259" s="12" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="E259" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A260" s="12" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B260" s="12" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="E260" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A261" s="12" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B261" s="12" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E261" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A262" s="12" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B262" s="12" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="E262" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A263" s="12" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B263" s="12" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="E263" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A264" s="12" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B264" s="12" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="E264" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A265" s="12" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B265" s="12" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="E265" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A266" s="12" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="B266" s="12" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="E266" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A267" s="12" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="B267" s="12" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="E267" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A268" s="12" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B268" s="12" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="E268" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A269" s="12" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B269" s="12" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="E269" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A270" s="12" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B270" s="12" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="E270" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A271" s="12" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B271" s="12" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="E271" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A272" s="12" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B272" s="12" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="E272" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A273" s="12" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B273" s="12" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="E273" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A274" s="12" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B274" s="12" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="E274" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A275" s="12" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B275" s="12" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="E275" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A276" s="12" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B276" s="12" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="E276" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A277" s="12" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B277" s="12" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="E277" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A278" s="12" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B278" s="12" t="s">
         <v>272</v>
       </c>
       <c r="E278" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A279" s="12" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="B279" s="12" t="s">
         <v>247</v>
       </c>
       <c r="E279" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A280" s="12" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="B280" s="12" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="E280" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A281" s="12" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B281" s="12" t="s">
         <v>295</v>
       </c>
       <c r="E281" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A282" s="12" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="B282" s="12" t="s">
         <v>263</v>
       </c>
       <c r="E282" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A283" s="12" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B283" s="12" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="E283" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A284" s="12" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="B284" s="12" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="E284" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A285" s="12" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="B285" s="12" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="E285" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A286" s="12" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B286" s="12" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="E286" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A287" s="12" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="B287" s="12" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="E287" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A288" s="12" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="B288" s="12" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="E288" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A289" s="12" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B289" s="12" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="E289" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A290" s="12" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B290" s="12" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="E290" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A291" s="12" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="B291" s="12" t="s">
         <v>247</v>
       </c>
       <c r="E291" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A292" s="12" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="B292" s="12" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="E292" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A293" s="12" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B293" s="12" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="E293" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A294" s="12" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B294" s="12" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="E294" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A295" s="12" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="B295" s="12" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="E295" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A296" s="12" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="B296" s="12" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="E296" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A297" s="12" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="B297" s="12" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="E297" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A298" s="12" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="B298" s="12" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="E298" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A299" s="12" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="B299" s="12" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="E299" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A300" s="12" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B300" s="12" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="E300" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A301" s="12" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="B301" s="12" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="E301" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A302" s="12" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="B302" s="12" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="E302" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A303" s="12" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="B303" s="12" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="E303" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A304" s="12" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="B304" s="12" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="E304" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A305" s="12" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="B305" s="12" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="E305" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A306" s="12" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="B306" s="12" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="E306" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A307" s="12" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="B307" s="12" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="E307" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A308" s="12" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="B308" s="12" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="E308" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A309" s="12" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="B309" s="12" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="E309" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A310" s="12" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="B310" s="12" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="E310" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A311" s="12" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="B311" s="12" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="E311" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A312" s="12" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="B312" s="12" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="E312" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A313" s="12" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="B313" s="12" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="E313" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A314" s="12" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="B314" s="12" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="E314" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A315" s="12" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="B315" s="12" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="E315" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A316" s="12" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="B316" s="12" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="E316" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A317" s="12" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="B317" s="12" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="E317" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A318" s="12" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B318" s="12" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E318" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A319" s="12" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B319" s="12" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="E319" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A320" s="12" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="B320" s="12" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="E320" s="12" t="s">
         <v>216</v>
@@ -6134,10 +6259,10 @@
     </row>
     <row r="321" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A321" s="12" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="B321" s="12" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="E321" s="12" t="s">
         <v>216</v>
@@ -6145,10 +6270,10 @@
     </row>
     <row r="322" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A322" s="12" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="B322" s="12" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="E322" s="12" t="s">
         <v>216</v>
@@ -6156,10 +6281,10 @@
     </row>
     <row r="323" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A323" s="12" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="B323" s="12" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="E323" s="12" t="s">
         <v>216</v>
@@ -6167,10 +6292,10 @@
     </row>
     <row r="324" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A324" s="12" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="B324" s="12" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="E324" s="12" t="s">
         <v>216</v>
@@ -6178,7 +6303,7 @@
     </row>
     <row r="325" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A325" s="12" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="B325" s="12" t="s">
         <v>272</v>
@@ -6189,10 +6314,10 @@
     </row>
     <row r="326" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A326" s="12" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="B326" s="12" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="E326" s="12" t="s">
         <v>218</v>
@@ -6200,10 +6325,10 @@
     </row>
     <row r="327" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A327" s="12" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B327" s="12" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="E327" s="12" t="s">
         <v>218</v>
@@ -6211,10 +6336,10 @@
     </row>
     <row r="328" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A328" s="12" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="B328" s="12" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="E328" s="12" t="s">
         <v>218</v>
@@ -6222,10 +6347,10 @@
     </row>
     <row r="329" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A329" s="12" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B329" s="12" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="E329" s="12" t="s">
         <v>218</v>
@@ -6233,10 +6358,10 @@
     </row>
     <row r="330" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A330" s="12" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="B330" s="12" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="E330" s="12" t="s">
         <v>218</v>
@@ -6244,10 +6369,10 @@
     </row>
     <row r="331" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A331" s="12" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="B331" s="12" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="E331" s="12" t="s">
         <v>218</v>
@@ -6255,10 +6380,10 @@
     </row>
     <row r="332" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A332" s="12" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="B332" s="12" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="E332" s="12" t="s">
         <v>220</v>
@@ -6266,10 +6391,10 @@
     </row>
     <row r="333" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A333" s="12" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="B333" s="12" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="E333" s="12" t="s">
         <v>220</v>
@@ -6277,10 +6402,10 @@
     </row>
     <row r="334" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A334" s="12" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B334" s="12" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="E334" s="12" t="s">
         <v>220</v>
@@ -6288,10 +6413,10 @@
     </row>
     <row r="335" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A335" s="12" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="B335" s="12" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="E335" s="12" t="s">
         <v>222</v>
@@ -6299,10 +6424,10 @@
     </row>
     <row r="336" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A336" s="12" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B336" s="12" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="E336" s="12" t="s">
         <v>222</v>
@@ -6310,10 +6435,10 @@
     </row>
     <row r="337" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A337" s="12" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="B337" s="12" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="E337" s="12" t="s">
         <v>224</v>
@@ -6321,10 +6446,10 @@
     </row>
     <row r="338" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A338" s="12" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B338" s="12" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="E338" s="12" t="s">
         <v>224</v>
@@ -6332,10 +6457,10 @@
     </row>
     <row r="339" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A339" s="12" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="B339" s="12" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="E339" s="12" t="s">
         <v>224</v>
@@ -6343,10 +6468,10 @@
     </row>
     <row r="340" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A340" s="12" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B340" s="12" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="E340" s="12" t="s">
         <v>226</v>
@@ -6354,10 +6479,10 @@
     </row>
     <row r="341" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A341" s="12" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="B341" s="12" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="E341" s="12" t="s">
         <v>226</v>
@@ -6365,10 +6490,10 @@
     </row>
     <row r="342" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A342" s="12" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="B342" s="12" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="E342" s="12" t="s">
         <v>226</v>
@@ -6376,10 +6501,10 @@
     </row>
     <row r="343" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A343" s="12" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="B343" s="12" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="E343" s="12" t="s">
         <v>226</v>
@@ -6387,10 +6512,10 @@
     </row>
     <row r="344" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A344" s="12" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B344" s="12" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="E344" s="12" t="s">
         <v>228</v>
@@ -6398,10 +6523,10 @@
     </row>
     <row r="345" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A345" s="12" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="B345" s="12" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="E345" s="12" t="s">
         <v>228</v>
@@ -6409,10 +6534,10 @@
     </row>
     <row r="346" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A346" s="12" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B346" s="12" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="E346" s="12" t="s">
         <v>228</v>
@@ -6420,10 +6545,10 @@
     </row>
     <row r="347" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A347" s="12" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B347" s="12" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="E347" s="12" t="s">
         <v>230</v>
@@ -6431,10 +6556,10 @@
     </row>
     <row r="348" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A348" s="12" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="B348" s="12" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="E348" s="12" t="s">
         <v>230</v>
@@ -6442,10 +6567,10 @@
     </row>
     <row r="349" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A349" s="12" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="B349" s="12" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="E349" s="12" t="s">
         <v>230</v>
@@ -6453,57 +6578,57 @@
     </row>
     <row r="350" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A350" s="12" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="B350" s="12" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="E350" s="12" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A351" s="12" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="B351" s="12" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="E351" s="12" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A352" s="12" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="B352" s="12" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="E352" s="12" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A353" s="12" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="B353" s="12" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="E353" s="12" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A354" s="12" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="B354" s="12" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="E354" s="12" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>